<commit_message>
Added latest HPS period to the periods table
</commit_message>
<xml_diff>
--- a/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
+++ b/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munchausend/GoogleDrive/MSc/Dissertation/Methods/DataStuff/table_details/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Survey_Social_Media_Compare/Methods/Scripts/Surveys/table_details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286F529F-8D1D-F143-AE3D-124D10C89D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA1C3A-E918-C34F-B963-BC7790745A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25340" yWindow="-9440" windowWidth="25100" windowHeight="14400" activeTab="2" xr2:uid="{ED69059E-CB6C-984A-904D-B506F2D7DD84}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="59">
   <si>
     <t>W29</t>
   </si>
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1680,6 +1680,21 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
+      <c r="E19" s="1">
+        <v>44328</v>
+      </c>
+      <c r="F19" s="1">
+        <v>44340</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="5"/>

</xml_diff>

<commit_message>
Vaccination data (Reddit & Twitter)
</commit_message>
<xml_diff>
--- a/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
+++ b/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Survey_Social_Media_Compare/Methods/Scripts/Surveys/table_details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEA1C3A-E918-C34F-B963-BC7790745A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3F6C0-D667-1547-BD2F-BBD2DAF232FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25340" yWindow="-9440" windowWidth="25100" windowHeight="14400" activeTab="2" xr2:uid="{ED69059E-CB6C-984A-904D-B506F2D7DD84}"/>
+    <workbookView xWindow="1900" yWindow="1260" windowWidth="25100" windowHeight="14400" activeTab="2" xr2:uid="{ED69059E-CB6C-984A-904D-B506F2D7DD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Axios_Ipsos" sheetId="1" r:id="rId1"/>
@@ -1134,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3062C6D8-6A7A-AA4F-9DEC-18A85AA1A337}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1700,6 +1700,7 @@
       <c r="D21" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added functionality to combine surveys with sm data
</commit_message>
<xml_diff>
--- a/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
+++ b/Methods/Scripts/Surveys/table_details/surveyPeriods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Survey_Social_Media_Compare/Methods/Scripts/Surveys/table_details/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F3F6C0-D667-1547-BD2F-BBD2DAF232FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120ED5EC-B13C-0E4E-BE5B-E80C15066292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1260" windowWidth="25100" windowHeight="14400" activeTab="2" xr2:uid="{ED69059E-CB6C-984A-904D-B506F2D7DD84}"/>
+    <workbookView xWindow="500" yWindow="1260" windowWidth="25100" windowHeight="14400" activeTab="2" xr2:uid="{ED69059E-CB6C-984A-904D-B506F2D7DD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Axios_Ipsos" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="60">
   <si>
     <t>W29</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>HPS_topic</t>
+  </si>
+  <si>
+    <t>P13</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3062C6D8-6A7A-AA4F-9DEC-18A85AA1A337}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1672,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1">
         <v>44337</v>

</xml_diff>